<commit_message>
Agregado análisis avanzado Planes
</commit_message>
<xml_diff>
--- a/data/Parametros.xlsx
+++ b/data/Parametros.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/1510d6d17ff2404d/99-DESARROLLO/Python/DataSmartExpress/App_DataSmart_Express/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="134" documentId="11_076110159C8BD21570149374E46859E1E1308BCD" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F7BD030F-8A87-431C-86F8-5A901F62961D}"/>
+  <xr:revisionPtr revIDLastSave="173" documentId="11_076110159C8BD21570149374E46859E1E1308BCD" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9A44873A-6057-4FD5-8721-330E1991B948}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="KPIS_FINANCIEROS" sheetId="2" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="47">
   <si>
     <t>GRUPO</t>
   </si>
@@ -151,34 +151,31 @@
     <t>TOTAL VENTAS</t>
   </si>
   <si>
+    <t>EXPORTAR_PDF</t>
+  </si>
+  <si>
+    <t>TARJETAS_KPI</t>
+  </si>
+  <si>
+    <t>ANALISIS_LENGUAJE</t>
+  </si>
+  <si>
+    <t>ANALISIS_AVANZADO</t>
+  </si>
+  <si>
+    <t>Free</t>
+  </si>
+  <si>
+    <t>Pro</t>
+  </si>
+  <si>
+    <t>Premium</t>
+  </si>
+  <si>
     <t>FUNCIONALIDAD</t>
   </si>
   <si>
-    <t>FREE</t>
-  </si>
-  <si>
-    <t>BASICO</t>
-  </si>
-  <si>
-    <t>PRO</t>
-  </si>
-  <si>
-    <t>PREMIUM</t>
-  </si>
-  <si>
-    <t>VER_KPIS</t>
-  </si>
-  <si>
-    <t>CONCLUSIONES</t>
-  </si>
-  <si>
-    <t>EXPORTAR_EXCEL</t>
-  </si>
-  <si>
-    <t>EXPORTAR_PDF</t>
-  </si>
-  <si>
-    <t>USOS_MAXIMOS</t>
+    <t>Basico</t>
   </si>
 </sst>
 </file>
@@ -202,7 +199,10 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -574,7 +574,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
@@ -878,37 +878,40 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9AD2B396-A028-439B-AD56-80C88A7629A9}">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.109375" customWidth="1"/>
+    <col min="2" max="2" width="18.44140625" customWidth="1"/>
+    <col min="3" max="3" width="19.77734375" customWidth="1"/>
+    <col min="4" max="4" width="20.44140625" customWidth="1"/>
+    <col min="5" max="5" width="20" customWidth="1"/>
+    <col min="6" max="6" width="19" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -925,7 +928,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="B3">
         <v>0</v>
@@ -942,7 +945,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="B4">
         <v>0</v>
@@ -959,7 +962,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="B5">
         <v>0</v>
@@ -974,24 +977,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>47</v>
-      </c>
-      <c r="B6">
-        <v>3</v>
-      </c>
-      <c r="C6">
-        <v>9999</v>
-      </c>
-      <c r="D6">
-        <v>9999</v>
-      </c>
-      <c r="E6">
-        <v>9999</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Versión Junio 15 de DataSmart Express
</commit_message>
<xml_diff>
--- a/data/Parametros.xlsx
+++ b/data/Parametros.xlsx
@@ -8,14 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/1510d6d17ff2404d/99-DESARROLLO/Python/DataSmartExpress/App_DataSmart_Express/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="173" documentId="11_076110159C8BD21570149374E46859E1E1308BCD" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9A44873A-6057-4FD5-8721-330E1991B948}"/>
+  <xr:revisionPtr revIDLastSave="449" documentId="11_076110159C8BD21570149374E46859E1E1308BCD" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{119863F1-5684-43DE-88AF-3F7608708AC0}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="KPIS_FINANCIEROS" sheetId="2" r:id="rId1"/>
-    <sheet name="TARJETAS" sheetId="3" r:id="rId2"/>
-    <sheet name="PLANES" sheetId="4" r:id="rId3"/>
+    <sheet name="GRAFICAS" sheetId="5" r:id="rId2"/>
+    <sheet name="TARJETAS" sheetId="3" r:id="rId3"/>
+    <sheet name="EN_ANALISIS" sheetId="6" r:id="rId4"/>
+    <sheet name="PLANES" sheetId="4" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="76">
   <si>
     <t>GRUPO</t>
   </si>
@@ -91,27 +93,18 @@
     <t>TOTAL VENTAS-TOTAL COSTO MERCANCIA VENDIDA-TOTAL GASTOS OPERACIONALES ADMINISTRACION-TOTAL GASTOS OPERACIONALES DE VENTAS+TOTAL INGRESOS NO OPERACIONALES-TOTAL GASTOS NO OPERACIONALES-TOTAL IMPUESTO DE RENTA</t>
   </si>
   <si>
-    <t>AMBOS</t>
-  </si>
-  <si>
     <t>MARGEN BRUTO %</t>
   </si>
   <si>
     <t>(TOTAL VENTAS-TOTAL COSTO MERCANCIA VENDIDA)/TOTAL VENTAS*100</t>
   </si>
   <si>
-    <t>DETALLE</t>
-  </si>
-  <si>
     <t>GASTOS OPERACIONALES %</t>
   </si>
   <si>
     <t>TOTAL GASTOS OPERACIONALES/TOTAL VENTAS*100</t>
   </si>
   <si>
-    <t>TARJETA</t>
-  </si>
-  <si>
     <t>RESULTADO OPERACIONAL %</t>
   </si>
   <si>
@@ -130,9 +123,6 @@
     <t>TOTAL RESULTADO DESPUES DE IMPUESTOS</t>
   </si>
   <si>
-    <t>VISIBLE_EN</t>
-  </si>
-  <si>
     <t>TIPO_DATO</t>
   </si>
   <si>
@@ -163,26 +153,125 @@
     <t>ANALISIS_AVANZADO</t>
   </si>
   <si>
+    <t>FUNCIONALIDAD</t>
+  </si>
+  <si>
+    <t>EXPORTAR_EXCEL</t>
+  </si>
+  <si>
     <t>Free</t>
   </si>
   <si>
+    <t>Basico</t>
+  </si>
+  <si>
     <t>Pro</t>
   </si>
   <si>
     <t>Premium</t>
   </si>
   <si>
-    <t>FUNCIONALIDAD</t>
-  </si>
-  <si>
-    <t>Basico</t>
+    <t>FILTRAR_CENTRO_COSTO</t>
+  </si>
+  <si>
+    <t>PG_ANUAL</t>
+  </si>
+  <si>
+    <t>MOSTRAR_EN_PG</t>
+  </si>
+  <si>
+    <t>TOTAL INGRESOS NO OPERACIONALES</t>
+  </si>
+  <si>
+    <t>GRAFICO</t>
+  </si>
+  <si>
+    <t>TIPO</t>
+  </si>
+  <si>
+    <t>BARRA</t>
+  </si>
+  <si>
+    <t>LINEAL</t>
+  </si>
+  <si>
+    <t>DESCRIPCION</t>
+  </si>
+  <si>
+    <t>Ventas por mes</t>
+  </si>
+  <si>
+    <t>Ventas Mensuales</t>
+  </si>
+  <si>
+    <t>Margen Bruto</t>
+  </si>
+  <si>
+    <t>Resultado Operacional</t>
+  </si>
+  <si>
+    <t>GRAFICAS</t>
+  </si>
+  <si>
+    <t>COLUMNA_TEXTO_EXTRA</t>
+  </si>
+  <si>
+    <t>MODO</t>
+  </si>
+  <si>
+    <t>Composición Costo de Ventas</t>
+  </si>
+  <si>
+    <t>MENSUAL</t>
+  </si>
+  <si>
+    <t>ANUAL</t>
+  </si>
+  <si>
+    <t>Distribución del costo entre cuentas que componen el CMV del mes seleccionado</t>
+  </si>
+  <si>
+    <t>COSTO MERCANCIA VENDIDA</t>
+  </si>
+  <si>
+    <t>TORTA</t>
+  </si>
+  <si>
+    <t>Gastos Operacionales Administracion</t>
+  </si>
+  <si>
+    <t>GASTOS OPERACIONALES ADMINISTRACION</t>
+  </si>
+  <si>
+    <t>Funcionalidad</t>
+  </si>
+  <si>
+    <t>Conclusiones mensuales</t>
+  </si>
+  <si>
+    <t>Comparativo mes anterior</t>
+  </si>
+  <si>
+    <t>Conclusiones anuales</t>
+  </si>
+  <si>
+    <t>Detectar alertas (&gt; umbral %)</t>
+  </si>
+  <si>
+    <t>Tendencias (3–6 meses)</t>
+  </si>
+  <si>
+    <t>Detección de anomalías estadísticas</t>
+  </si>
+  <si>
+    <t>Resumen narrativo con GPT</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -203,6 +292,13 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="7"/>
+      <color rgb="FF31333F"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -251,7 +347,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -267,6 +363,22 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -572,10 +684,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:I10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -583,11 +695,11 @@
     <col min="1" max="1" width="31.88671875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="86.33203125" style="3" customWidth="1"/>
     <col min="3" max="3" width="37.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.77734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.109375" customWidth="1"/>
+    <col min="5" max="5" width="16.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
@@ -597,14 +709,26 @@
       <c r="C1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>31</v>
+      <c r="D1" s="4" t="s">
+        <v>28</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+        <v>46</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="H1" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="I1" s="7" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -615,30 +739,54 @@
         <v>8</v>
       </c>
       <c r="D2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+      <c r="H2">
+        <v>1</v>
+      </c>
+      <c r="I2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
         <v>18</v>
       </c>
-      <c r="E2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+      <c r="B3" s="3" t="s">
         <v>19</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>20</v>
       </c>
       <c r="C3" t="s">
         <v>8</v>
       </c>
       <c r="D3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E3" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+        <v>30</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="F3">
+        <v>1</v>
+      </c>
+      <c r="G3">
+        <v>1</v>
+      </c>
+      <c r="H3">
+        <v>1</v>
+      </c>
+      <c r="I3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -649,30 +797,54 @@
         <v>9</v>
       </c>
       <c r="D4" t="s">
-        <v>18</v>
-      </c>
-      <c r="E4" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+        <v>29</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+      <c r="G4">
+        <v>1</v>
+      </c>
+      <c r="H4">
+        <v>1</v>
+      </c>
+      <c r="I4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C5" t="s">
         <v>2</v>
       </c>
       <c r="D5" t="s">
-        <v>24</v>
-      </c>
-      <c r="E5" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+        <v>30</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="F5">
+        <v>1</v>
+      </c>
+      <c r="G5">
+        <v>1</v>
+      </c>
+      <c r="H5">
+        <v>1</v>
+      </c>
+      <c r="I5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -683,30 +855,54 @@
         <v>9</v>
       </c>
       <c r="D6" t="s">
-        <v>21</v>
-      </c>
-      <c r="E6" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+        <v>29</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6">
+        <v>1</v>
+      </c>
+      <c r="I6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C7" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D7" t="s">
-        <v>24</v>
-      </c>
-      <c r="E7" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+        <v>30</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="H7">
+        <v>1</v>
+      </c>
+      <c r="I7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>3</v>
       </c>
@@ -717,13 +913,25 @@
         <v>10</v>
       </c>
       <c r="D8" t="s">
-        <v>21</v>
-      </c>
-      <c r="E8" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+        <v>29</v>
+      </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="G8">
+        <v>0</v>
+      </c>
+      <c r="H8">
+        <v>1</v>
+      </c>
+      <c r="I8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>4</v>
       </c>
@@ -734,27 +942,51 @@
         <v>11</v>
       </c>
       <c r="D9" t="s">
-        <v>21</v>
-      </c>
-      <c r="E9" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+        <v>29</v>
+      </c>
+      <c r="E9">
+        <v>1</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
+      <c r="G9">
+        <v>1</v>
+      </c>
+      <c r="H9">
+        <v>1</v>
+      </c>
+      <c r="I9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C10" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D10" t="s">
-        <v>24</v>
-      </c>
-      <c r="E10" t="s">
-        <v>33</v>
+        <v>29</v>
+      </c>
+      <c r="E10">
+        <v>1</v>
+      </c>
+      <c r="F10">
+        <v>1</v>
+      </c>
+      <c r="G10">
+        <v>1</v>
+      </c>
+      <c r="H10">
+        <v>1</v>
+      </c>
+      <c r="I10">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -763,45 +995,314 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA1A63FD-C732-483A-BB65-70FBDDBA7676}">
+  <dimension ref="A1:L6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L5" sqref="L5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="28.88671875" customWidth="1"/>
+    <col min="7" max="8" width="23.109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="3.88671875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A1" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="I1" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="J1" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="K1" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="L1" s="7" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D2" t="s">
+        <v>33</v>
+      </c>
+      <c r="E2" t="s">
+        <v>62</v>
+      </c>
+      <c r="F2" t="s">
+        <v>53</v>
+      </c>
+      <c r="G2" t="s">
+        <v>29</v>
+      </c>
+      <c r="I2">
+        <v>0</v>
+      </c>
+      <c r="J2">
+        <v>1</v>
+      </c>
+      <c r="K2">
+        <v>1</v>
+      </c>
+      <c r="L2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E3" t="s">
+        <v>62</v>
+      </c>
+      <c r="F3" t="s">
+        <v>55</v>
+      </c>
+      <c r="G3" t="s">
+        <v>29</v>
+      </c>
+      <c r="H3" t="s">
+        <v>18</v>
+      </c>
+      <c r="I3">
+        <v>0</v>
+      </c>
+      <c r="J3">
+        <v>1</v>
+      </c>
+      <c r="K3">
+        <v>1</v>
+      </c>
+      <c r="L3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>56</v>
+      </c>
+      <c r="C4" t="s">
+        <v>51</v>
+      </c>
+      <c r="D4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" t="s">
+        <v>62</v>
+      </c>
+      <c r="F4" t="s">
+        <v>56</v>
+      </c>
+      <c r="G4" t="s">
+        <v>29</v>
+      </c>
+      <c r="I4">
+        <v>0</v>
+      </c>
+      <c r="J4">
+        <v>0</v>
+      </c>
+      <c r="K4">
+        <v>1</v>
+      </c>
+      <c r="L4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A5" s="9">
+        <v>4</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="E5" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="F5" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="G5" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="I5">
+        <v>0</v>
+      </c>
+      <c r="J5">
+        <v>0</v>
+      </c>
+      <c r="K5">
+        <v>1</v>
+      </c>
+      <c r="L5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>66</v>
+      </c>
+      <c r="C6" t="s">
+        <v>50</v>
+      </c>
+      <c r="D6" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="E6" t="s">
+        <v>61</v>
+      </c>
+      <c r="F6" t="s">
+        <v>66</v>
+      </c>
+      <c r="G6" t="s">
+        <v>29</v>
+      </c>
+      <c r="I6">
+        <v>0</v>
+      </c>
+      <c r="J6">
+        <v>0</v>
+      </c>
+      <c r="K6">
+        <v>1</v>
+      </c>
+      <c r="L6">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC8F708E-264A-4BE0-B59B-C2CBA66A93D2}">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:H13"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:H4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="31.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>35</v>
-      </c>
-      <c r="B1" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="C1" t="s">
-        <v>36</v>
-      </c>
-      <c r="D1" t="s">
+      <c r="C1" s="6" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D1" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="H1" s="7" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="C2" t="s">
         <v>0</v>
       </c>
       <c r="D2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+        <v>29</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+      <c r="H2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -812,10 +1313,22 @@
         <v>0</v>
       </c>
       <c r="D3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+        <v>29</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="F3">
+        <v>1</v>
+      </c>
+      <c r="G3">
+        <v>1</v>
+      </c>
+      <c r="H3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -826,24 +1339,48 @@
         <v>5</v>
       </c>
       <c r="D4" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+        <v>29</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+      <c r="G4">
+        <v>1</v>
+      </c>
+      <c r="H4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C5" t="s">
         <v>5</v>
       </c>
       <c r="D5" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+        <v>30</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="F5">
+        <v>1</v>
+      </c>
+      <c r="G5">
+        <v>1</v>
+      </c>
+      <c r="H5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -854,10 +1391,22 @@
         <v>5</v>
       </c>
       <c r="D6" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+        <v>29</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>1</v>
+      </c>
+      <c r="H6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -868,7 +1417,330 @@
         <v>5</v>
       </c>
       <c r="D7" t="s">
-        <v>33</v>
+        <v>29</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <v>1</v>
+      </c>
+      <c r="H7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" t="s">
+        <v>5</v>
+      </c>
+      <c r="D8" t="s">
+        <v>30</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="G8">
+        <v>1</v>
+      </c>
+      <c r="H8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>47</v>
+      </c>
+      <c r="C9" t="s">
+        <v>0</v>
+      </c>
+      <c r="D9" t="s">
+        <v>29</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="F9">
+        <v>1</v>
+      </c>
+      <c r="G9">
+        <v>1</v>
+      </c>
+      <c r="H9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" t="s">
+        <v>0</v>
+      </c>
+      <c r="D10" t="s">
+        <v>29</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <v>1</v>
+      </c>
+      <c r="G10">
+        <v>1</v>
+      </c>
+      <c r="H10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>3</v>
+      </c>
+      <c r="C11" t="s">
+        <v>5</v>
+      </c>
+      <c r="D11" t="s">
+        <v>29</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+      <c r="F11">
+        <v>1</v>
+      </c>
+      <c r="G11">
+        <v>1</v>
+      </c>
+      <c r="H11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>11</v>
+      </c>
+      <c r="C12" t="s">
+        <v>0</v>
+      </c>
+      <c r="D12" t="s">
+        <v>29</v>
+      </c>
+      <c r="E12">
+        <v>0</v>
+      </c>
+      <c r="F12">
+        <v>0</v>
+      </c>
+      <c r="G12">
+        <v>1</v>
+      </c>
+      <c r="H12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>4</v>
+      </c>
+      <c r="C13" t="s">
+        <v>5</v>
+      </c>
+      <c r="D13" t="s">
+        <v>29</v>
+      </c>
+      <c r="E13">
+        <v>0</v>
+      </c>
+      <c r="F13">
+        <v>1</v>
+      </c>
+      <c r="G13">
+        <v>1</v>
+      </c>
+      <c r="H13">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC7CFF8A-3790-4A69-BD86-157F17280CF7}">
+  <dimension ref="A1:E8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="15.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="41.109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A2" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="B2" s="11">
+        <v>1</v>
+      </c>
+      <c r="C2" s="11">
+        <v>1</v>
+      </c>
+      <c r="D2" s="11">
+        <v>1</v>
+      </c>
+      <c r="E2" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A3" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="B3" s="11">
+        <v>0</v>
+      </c>
+      <c r="C3" s="11">
+        <v>0</v>
+      </c>
+      <c r="D3" s="11">
+        <v>1</v>
+      </c>
+      <c r="E3" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A4" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="B4" s="11">
+        <v>0</v>
+      </c>
+      <c r="C4" s="11">
+        <v>0</v>
+      </c>
+      <c r="D4" s="11">
+        <v>1</v>
+      </c>
+      <c r="E4" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A5" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="B5" s="11">
+        <v>0</v>
+      </c>
+      <c r="C5" s="11">
+        <v>0</v>
+      </c>
+      <c r="D5" s="11">
+        <v>1</v>
+      </c>
+      <c r="E5" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A6" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="B6" s="11">
+        <v>0</v>
+      </c>
+      <c r="C6" s="11">
+        <v>0</v>
+      </c>
+      <c r="D6" s="11">
+        <v>0</v>
+      </c>
+      <c r="E6" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A7" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="B7" s="11">
+        <v>0</v>
+      </c>
+      <c r="C7" s="11">
+        <v>0</v>
+      </c>
+      <c r="D7" s="11">
+        <v>0</v>
+      </c>
+      <c r="E7" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A8" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="B8" s="11">
+        <v>0</v>
+      </c>
+      <c r="C8" s="11">
+        <v>0</v>
+      </c>
+      <c r="D8" s="11">
+        <v>0</v>
+      </c>
+      <c r="E8" s="11">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -876,11 +1748,13 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9AD2B396-A028-439B-AD56-80C88A7629A9}">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -889,35 +1763,34 @@
     <col min="3" max="3" width="19.77734375" customWidth="1"/>
     <col min="4" max="4" width="20.44140625" customWidth="1"/>
     <col min="5" max="5" width="20" customWidth="1"/>
-    <col min="6" max="6" width="19" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="B1" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="D1" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="C1" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="D1" s="5" t="s">
+      <c r="E1" s="5" t="s">
         <v>43</v>
-      </c>
-      <c r="E1" s="5" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="B2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -928,10 +1801,10 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="B3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C3">
         <v>1</v>
@@ -945,13 +1818,13 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="B4">
         <v>0</v>
       </c>
       <c r="C4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D4">
         <v>1</v>
@@ -962,7 +1835,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B5">
         <v>0</v>
@@ -971,9 +1844,77 @@
         <v>0</v>
       </c>
       <c r="D5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>34</v>
+      </c>
+      <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>39</v>
+      </c>
+      <c r="B7">
+        <v>0</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>45</v>
+      </c>
+      <c r="B8">
+        <v>0</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>57</v>
+      </c>
+      <c r="B9">
+        <v>0</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="E9">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
🔄 Subida versión actualizada con flujo de recuperación por Supabase
</commit_message>
<xml_diff>
--- a/data/Parametros.xlsx
+++ b/data/Parametros.xlsx
@@ -8,16 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/1510d6d17ff2404d/99-DESARROLLO/Python/DataSmartExpress/App_DataSmart_Express/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="449" documentId="11_076110159C8BD21570149374E46859E1E1308BCD" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{119863F1-5684-43DE-88AF-3F7608708AC0}"/>
+  <xr:revisionPtr revIDLastSave="491" documentId="11_076110159C8BD21570149374E46859E1E1308BCD" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F806B7BE-5BA5-477D-AD0C-964F3697CAD0}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="KPIS_FINANCIEROS" sheetId="2" r:id="rId1"/>
     <sheet name="GRAFICAS" sheetId="5" r:id="rId2"/>
-    <sheet name="TARJETAS" sheetId="3" r:id="rId3"/>
-    <sheet name="EN_ANALISIS" sheetId="6" r:id="rId4"/>
-    <sheet name="PLANES" sheetId="4" r:id="rId5"/>
+    <sheet name="COMENTARIOS_GRAFICAS" sheetId="7" r:id="rId3"/>
+    <sheet name="TARJETAS" sheetId="3" r:id="rId4"/>
+    <sheet name="EN_ANALISIS" sheetId="6" r:id="rId5"/>
+    <sheet name="PLANES" sheetId="4" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="80">
   <si>
     <t>GRUPO</t>
   </si>
@@ -265,6 +266,18 @@
   </si>
   <si>
     <t>Resumen narrativo con GPT</t>
+  </si>
+  <si>
+    <t>Comentario GPT</t>
+  </si>
+  <si>
+    <t>TIPO_COMENTARIO</t>
+  </si>
+  <si>
+    <t>Comentario Python</t>
+  </si>
+  <si>
+    <t>GRAFICAS_INTELIGENTES</t>
   </si>
 </sst>
 </file>
@@ -347,7 +360,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -380,6 +393,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -687,7 +701,7 @@
   <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="B6" sqref="A6:XFD6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -999,7 +1013,7 @@
   <dimension ref="A1:L6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L5" sqref="L5"/>
+      <selection sqref="A1:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1238,6 +1252,75 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E68DE59-992B-4058-A203-82C1DEABD0B6}">
+  <dimension ref="A1:E3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="21" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>78</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>76</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC8F708E-264A-4BE0-B59B-C2CBA66A93D2}">
   <dimension ref="A1:H13"/>
   <sheetViews>
@@ -1594,11 +1677,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC7CFF8A-3790-4A69-BD86-157F17280CF7}">
   <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
@@ -1692,7 +1775,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="9" t="s">
         <v>73</v>
       </c>
@@ -1709,7 +1792,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="9" t="s">
         <v>74</v>
       </c>
@@ -1748,17 +1831,17 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9AD2B396-A028-439B-AD56-80C88A7629A9}">
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="22.109375" customWidth="1"/>
+    <col min="1" max="1" width="22.109375" style="12" customWidth="1"/>
     <col min="2" max="2" width="18.44140625" customWidth="1"/>
     <col min="3" max="3" width="19.77734375" customWidth="1"/>
     <col min="4" max="4" width="20.44140625" customWidth="1"/>
@@ -1783,7 +1866,7 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="A2" s="12" t="s">
         <v>44</v>
       </c>
       <c r="B2">
@@ -1800,7 +1883,7 @@
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+      <c r="A3" s="12" t="s">
         <v>35</v>
       </c>
       <c r="B3">
@@ -1817,7 +1900,7 @@
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+      <c r="A4" s="12" t="s">
         <v>36</v>
       </c>
       <c r="B4">
@@ -1834,7 +1917,7 @@
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+      <c r="A5" s="12" t="s">
         <v>37</v>
       </c>
       <c r="B5">
@@ -1851,7 +1934,7 @@
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+      <c r="A6" s="12" t="s">
         <v>34</v>
       </c>
       <c r="B6">
@@ -1868,7 +1951,7 @@
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
+      <c r="A7" s="12" t="s">
         <v>39</v>
       </c>
       <c r="B7">
@@ -1885,7 +1968,7 @@
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
+      <c r="A8" s="12" t="s">
         <v>45</v>
       </c>
       <c r="B8">
@@ -1902,7 +1985,7 @@
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
+      <c r="A9" s="12" t="s">
         <v>57</v>
       </c>
       <c r="B9">
@@ -1915,6 +1998,23 @@
         <v>1</v>
       </c>
       <c r="E9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10" s="12" t="s">
+        <v>79</v>
+      </c>
+      <c r="B10">
+        <v>0</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Restauración desde backup y correcciones de restablecer contraseña
</commit_message>
<xml_diff>
--- a/data/Parametros.xlsx
+++ b/data/Parametros.xlsx
@@ -8,16 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/1510d6d17ff2404d/99-DESARROLLO/Python/DataSmartExpress/App_DataSmart_Express/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="449" documentId="11_076110159C8BD21570149374E46859E1E1308BCD" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{119863F1-5684-43DE-88AF-3F7608708AC0}"/>
+  <xr:revisionPtr revIDLastSave="491" documentId="11_076110159C8BD21570149374E46859E1E1308BCD" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F806B7BE-5BA5-477D-AD0C-964F3697CAD0}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="KPIS_FINANCIEROS" sheetId="2" r:id="rId1"/>
     <sheet name="GRAFICAS" sheetId="5" r:id="rId2"/>
-    <sheet name="TARJETAS" sheetId="3" r:id="rId3"/>
-    <sheet name="EN_ANALISIS" sheetId="6" r:id="rId4"/>
-    <sheet name="PLANES" sheetId="4" r:id="rId5"/>
+    <sheet name="COMENTARIOS_GRAFICAS" sheetId="7" r:id="rId3"/>
+    <sheet name="TARJETAS" sheetId="3" r:id="rId4"/>
+    <sheet name="EN_ANALISIS" sheetId="6" r:id="rId5"/>
+    <sheet name="PLANES" sheetId="4" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="80">
   <si>
     <t>GRUPO</t>
   </si>
@@ -265,6 +266,18 @@
   </si>
   <si>
     <t>Resumen narrativo con GPT</t>
+  </si>
+  <si>
+    <t>Comentario GPT</t>
+  </si>
+  <si>
+    <t>TIPO_COMENTARIO</t>
+  </si>
+  <si>
+    <t>Comentario Python</t>
+  </si>
+  <si>
+    <t>GRAFICAS_INTELIGENTES</t>
   </si>
 </sst>
 </file>
@@ -347,7 +360,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -380,6 +393,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -687,7 +701,7 @@
   <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="B6" sqref="A6:XFD6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -999,7 +1013,7 @@
   <dimension ref="A1:L6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L5" sqref="L5"/>
+      <selection sqref="A1:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1238,6 +1252,75 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E68DE59-992B-4058-A203-82C1DEABD0B6}">
+  <dimension ref="A1:E3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="21" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>78</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>76</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC8F708E-264A-4BE0-B59B-C2CBA66A93D2}">
   <dimension ref="A1:H13"/>
   <sheetViews>
@@ -1594,11 +1677,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC7CFF8A-3790-4A69-BD86-157F17280CF7}">
   <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
@@ -1692,7 +1775,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="9" t="s">
         <v>73</v>
       </c>
@@ -1709,7 +1792,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="9" t="s">
         <v>74</v>
       </c>
@@ -1748,17 +1831,17 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9AD2B396-A028-439B-AD56-80C88A7629A9}">
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="22.109375" customWidth="1"/>
+    <col min="1" max="1" width="22.109375" style="12" customWidth="1"/>
     <col min="2" max="2" width="18.44140625" customWidth="1"/>
     <col min="3" max="3" width="19.77734375" customWidth="1"/>
     <col min="4" max="4" width="20.44140625" customWidth="1"/>
@@ -1783,7 +1866,7 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="A2" s="12" t="s">
         <v>44</v>
       </c>
       <c r="B2">
@@ -1800,7 +1883,7 @@
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+      <c r="A3" s="12" t="s">
         <v>35</v>
       </c>
       <c r="B3">
@@ -1817,7 +1900,7 @@
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+      <c r="A4" s="12" t="s">
         <v>36</v>
       </c>
       <c r="B4">
@@ -1834,7 +1917,7 @@
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+      <c r="A5" s="12" t="s">
         <v>37</v>
       </c>
       <c r="B5">
@@ -1851,7 +1934,7 @@
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+      <c r="A6" s="12" t="s">
         <v>34</v>
       </c>
       <c r="B6">
@@ -1868,7 +1951,7 @@
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
+      <c r="A7" s="12" t="s">
         <v>39</v>
       </c>
       <c r="B7">
@@ -1885,7 +1968,7 @@
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
+      <c r="A8" s="12" t="s">
         <v>45</v>
       </c>
       <c r="B8">
@@ -1902,7 +1985,7 @@
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
+      <c r="A9" s="12" t="s">
         <v>57</v>
       </c>
       <c r="B9">
@@ -1915,6 +1998,23 @@
         <v>1</v>
       </c>
       <c r="E9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10" s="12" t="s">
+        <v>79</v>
+      </c>
+      <c r="B10">
+        <v>0</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
🛠 Junio 30 - 1
</commit_message>
<xml_diff>
--- a/data/Parametros.xlsx
+++ b/data/Parametros.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/1510d6d17ff2404d/99-DESARROLLO/Python/DataSmartExpress/App_DataSmart_Express/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="491" documentId="11_076110159C8BD21570149374E46859E1E1308BCD" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F806B7BE-5BA5-477D-AD0C-964F3697CAD0}"/>
+  <xr:revisionPtr revIDLastSave="547" documentId="11_076110159C8BD21570149374E46859E1E1308BCD" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1C800B12-055A-4FF8-A6C3-C155C4AE9FB4}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="KPIS_FINANCIEROS" sheetId="2" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="81">
   <si>
     <t>GRUPO</t>
   </si>
@@ -278,6 +278,9 @@
   </si>
   <si>
     <t>GRAFICAS_INTELIGENTES</t>
+  </si>
+  <si>
+    <t>Premium_trial</t>
   </si>
 </sst>
 </file>
@@ -322,7 +325,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -356,11 +359,20 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -394,6 +406,15 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -698,10 +719,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:I10"/>
+  <dimension ref="A1:J10"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B6" sqref="A6:XFD6"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -713,7 +734,7 @@
     <col min="5" max="5" width="16.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
@@ -741,8 +762,11 @@
       <c r="I1" s="7" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J1" s="15" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -770,8 +794,11 @@
       <c r="I2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>18</v>
       </c>
@@ -799,8 +826,11 @@
       <c r="I3">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -828,8 +858,11 @@
       <c r="I4">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>20</v>
       </c>
@@ -857,8 +890,11 @@
       <c r="I5">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="J5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -886,8 +922,11 @@
       <c r="I6">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>22</v>
       </c>
@@ -915,8 +954,11 @@
       <c r="I7">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="J7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>3</v>
       </c>
@@ -944,8 +986,11 @@
       <c r="I8">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="J8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>4</v>
       </c>
@@ -973,8 +1018,11 @@
       <c r="I9">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>25</v>
       </c>
@@ -1000,6 +1048,9 @@
         <v>1</v>
       </c>
       <c r="I10">
+        <v>1</v>
+      </c>
+      <c r="J10">
         <v>1</v>
       </c>
     </row>
@@ -1010,10 +1061,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA1A63FD-C732-483A-BB65-70FBDDBA7676}">
-  <dimension ref="A1:L6"/>
+  <dimension ref="A1:M6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD3"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="M5" sqref="M5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1030,7 +1081,7 @@
     <col min="11" max="11" width="8.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
         <v>31</v>
       </c>
@@ -1067,8 +1118,11 @@
       <c r="L1" s="7" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M1" s="14" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1102,8 +1156,11 @@
       <c r="L2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1140,8 +1197,11 @@
       <c r="L3">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1175,8 +1235,11 @@
       <c r="L4">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="M4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A5" s="9">
         <v>4</v>
       </c>
@@ -1210,8 +1273,11 @@
       <c r="L5">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1243,6 +1309,9 @@
         <v>1</v>
       </c>
       <c r="L6">
+        <v>1</v>
+      </c>
+      <c r="M6">
         <v>1</v>
       </c>
     </row>
@@ -1253,10 +1322,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E68DE59-992B-4058-A203-82C1DEABD0B6}">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1264,7 +1333,7 @@
     <col min="1" max="1" width="21" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
         <v>77</v>
       </c>
@@ -1280,8 +1349,11 @@
       <c r="E1" s="7" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F1" s="14" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>78</v>
       </c>
@@ -1297,8 +1369,11 @@
       <c r="E2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>76</v>
       </c>
@@ -1312,6 +1387,9 @@
         <v>0</v>
       </c>
       <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="F3">
         <v>1</v>
       </c>
     </row>
@@ -1322,10 +1400,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC8F708E-264A-4BE0-B59B-C2CBA66A93D2}">
-  <dimension ref="A1:H13"/>
+  <dimension ref="A1:I13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:H4"/>
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1333,7 +1411,7 @@
     <col min="2" max="2" width="31.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
         <v>31</v>
       </c>
@@ -1358,8 +1436,11 @@
       <c r="H1" s="7" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I1" s="14" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1384,8 +1465,11 @@
       <c r="H2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1410,8 +1494,11 @@
       <c r="H3">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1436,8 +1523,11 @@
       <c r="H4">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1462,8 +1552,11 @@
       <c r="H5">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1488,8 +1581,11 @@
       <c r="H6">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1514,8 +1610,11 @@
       <c r="H7">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1540,8 +1639,11 @@
       <c r="H8">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1566,8 +1668,11 @@
       <c r="H9">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1592,8 +1697,11 @@
       <c r="H10">
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1618,8 +1726,11 @@
       <c r="H11">
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1644,8 +1755,11 @@
       <c r="H12">
         <v>1</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1668,6 +1782,9 @@
         <v>1</v>
       </c>
       <c r="H13">
+        <v>1</v>
+      </c>
+      <c r="I13">
         <v>1</v>
       </c>
     </row>
@@ -1679,10 +1796,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC7CFF8A-3790-4A69-BD86-157F17280CF7}">
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="15.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1690,7 +1807,7 @@
     <col min="1" max="1" width="41.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="8" t="s">
         <v>68</v>
       </c>
@@ -1706,8 +1823,11 @@
       <c r="E1" s="8" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="F1" s="8" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="9" t="s">
         <v>69</v>
       </c>
@@ -1723,8 +1843,11 @@
       <c r="E2" s="11">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="F2" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="9" t="s">
         <v>70</v>
       </c>
@@ -1740,8 +1863,11 @@
       <c r="E3" s="11">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="F3" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="9" t="s">
         <v>71</v>
       </c>
@@ -1757,8 +1883,11 @@
       <c r="E4" s="11">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="F4" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="9" t="s">
         <v>72</v>
       </c>
@@ -1774,8 +1903,11 @@
       <c r="E5" s="11">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F5" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="9" t="s">
         <v>73</v>
       </c>
@@ -1791,8 +1923,11 @@
       <c r="E6" s="11">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F6" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="9" t="s">
         <v>74</v>
       </c>
@@ -1808,8 +1943,11 @@
       <c r="E7" s="11">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="F7" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="9" t="s">
         <v>75</v>
       </c>
@@ -1823,6 +1961,9 @@
         <v>0</v>
       </c>
       <c r="E8" s="11">
+        <v>1</v>
+      </c>
+      <c r="F8" s="11">
         <v>1</v>
       </c>
     </row>
@@ -1833,10 +1974,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9AD2B396-A028-439B-AD56-80C88A7629A9}">
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1846,9 +1987,10 @@
     <col min="3" max="3" width="19.77734375" customWidth="1"/>
     <col min="4" max="4" width="20.44140625" customWidth="1"/>
     <col min="5" max="5" width="20" customWidth="1"/>
+    <col min="6" max="6" width="12.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>38</v>
       </c>
@@ -1864,8 +2006,11 @@
       <c r="E1" s="5" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F1" s="13" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="12" t="s">
         <v>44</v>
       </c>
@@ -1881,8 +2026,11 @@
       <c r="E2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="12" t="s">
         <v>35</v>
       </c>
@@ -1898,8 +2046,11 @@
       <c r="E3">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="12" t="s">
         <v>36</v>
       </c>
@@ -1915,8 +2066,11 @@
       <c r="E4">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="12" t="s">
         <v>37</v>
       </c>
@@ -1932,8 +2086,11 @@
       <c r="E5">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="12" t="s">
         <v>34</v>
       </c>
@@ -1949,8 +2106,11 @@
       <c r="E6">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="12" t="s">
         <v>39</v>
       </c>
@@ -1966,8 +2126,11 @@
       <c r="E7">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="12" t="s">
         <v>45</v>
       </c>
@@ -1983,8 +2146,11 @@
       <c r="E8">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="12" t="s">
         <v>57</v>
       </c>
@@ -2000,8 +2166,11 @@
       <c r="E9">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="12" t="s">
         <v>79</v>
       </c>
@@ -2015,6 +2184,9 @@
         <v>0</v>
       </c>
       <c r="E10">
+        <v>1</v>
+      </c>
+      <c r="F10">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
🛠 Julio 8 - 1
</commit_message>
<xml_diff>
--- a/data/Parametros.xlsx
+++ b/data/Parametros.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28925"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/1510d6d17ff2404d/99-DESARROLLO/Python/DataSmartExpress/App_DataSmart_Express/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\00-OneDrive\OneDrive\99-DESARROLLO\Python\DataSmartExpress\App_DataSmart_Express\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="547" documentId="11_076110159C8BD21570149374E46859E1E1308BCD" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1C800B12-055A-4FF8-A6C3-C155C4AE9FB4}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B72BE30E-4700-4877-934F-EAACCF4CDCCF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="KPIS_FINANCIEROS" sheetId="2" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="95">
   <si>
     <t>GRUPO</t>
   </si>
@@ -281,6 +281,48 @@
   </si>
   <si>
     <t>Premium_trial</t>
+  </si>
+  <si>
+    <t>Filtrar por centro de costos</t>
+  </si>
+  <si>
+    <t>Tarjetas con indicadores clave</t>
+  </si>
+  <si>
+    <t>Análisis en lenguaje natural</t>
+  </si>
+  <si>
+    <t>Exportar reportes a PDF</t>
+  </si>
+  <si>
+    <t>Análisis Avanzado AI</t>
+  </si>
+  <si>
+    <t>Exportar reportes a Excel</t>
+  </si>
+  <si>
+    <t>Estado de Resultados Anual</t>
+  </si>
+  <si>
+    <t>Gráficas de Indicadores</t>
+  </si>
+  <si>
+    <t>Gráficas de Indicadores con Análisis AI</t>
+  </si>
+  <si>
+    <t>Análisis automático con resumen mensual</t>
+  </si>
+  <si>
+    <t>Comparativo automático entre meses</t>
+  </si>
+  <si>
+    <t>Alertas de KPIs por encima del umbral</t>
+  </si>
+  <si>
+    <t>Conclusiones inteligentes con IA</t>
+  </si>
+  <si>
+    <t>Tendencias 3 - 6 meses</t>
   </si>
 </sst>
 </file>
@@ -372,7 +414,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -406,15 +448,19 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -721,7 +767,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:J10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
@@ -1796,43 +1842,44 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC7CFF8A-3790-4A69-BD86-157F17280CF7}">
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:G8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="15.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="41.109375" customWidth="1"/>
+    <col min="1" max="2" width="41.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="8" t="s">
         <v>68</v>
       </c>
       <c r="B1" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="C1" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="D1" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="E1" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="F1" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="G1" s="8" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="9" t="s">
         <v>69</v>
       </c>
-      <c r="B2" s="11">
-        <v>1</v>
+      <c r="B2" s="9" t="s">
+        <v>90</v>
       </c>
       <c r="C2" s="11">
         <v>1</v>
@@ -1846,19 +1893,22 @@
       <c r="F2" s="11">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G2" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="9" t="s">
         <v>70</v>
       </c>
-      <c r="B3" s="11">
-        <v>0</v>
+      <c r="B3" s="9" t="s">
+        <v>91</v>
       </c>
       <c r="C3" s="11">
         <v>0</v>
       </c>
       <c r="D3" s="11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E3" s="11">
         <v>1</v>
@@ -1866,19 +1916,22 @@
       <c r="F3" s="11">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G3" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="B4" s="11">
-        <v>0</v>
+      <c r="B4" s="9" t="s">
+        <v>71</v>
       </c>
       <c r="C4" s="11">
         <v>0</v>
       </c>
       <c r="D4" s="11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E4" s="11">
         <v>1</v>
@@ -1886,19 +1939,22 @@
       <c r="F4" s="11">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G4" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="9" t="s">
         <v>72</v>
       </c>
-      <c r="B5" s="11">
-        <v>0</v>
+      <c r="B5" s="9" t="s">
+        <v>92</v>
       </c>
       <c r="C5" s="11">
         <v>0</v>
       </c>
       <c r="D5" s="11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E5" s="11">
         <v>1</v>
@@ -1906,13 +1962,16 @@
       <c r="F5" s="11">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G5" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="9" t="s">
         <v>73</v>
       </c>
-      <c r="B6" s="11">
-        <v>0</v>
+      <c r="B6" s="9" t="s">
+        <v>94</v>
       </c>
       <c r="C6" s="11">
         <v>0</v>
@@ -1921,18 +1980,21 @@
         <v>0</v>
       </c>
       <c r="E6" s="11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F6" s="11">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G6" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="9" t="s">
         <v>74</v>
       </c>
-      <c r="B7" s="11">
-        <v>0</v>
+      <c r="B7" s="9" t="s">
+        <v>74</v>
       </c>
       <c r="C7" s="11">
         <v>0</v>
@@ -1941,18 +2003,21 @@
         <v>0</v>
       </c>
       <c r="E7" s="11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F7" s="11">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G7" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="9" t="s">
         <v>75</v>
       </c>
-      <c r="B8" s="11">
-        <v>0</v>
+      <c r="B8" s="9" t="s">
+        <v>93</v>
       </c>
       <c r="C8" s="11">
         <v>0</v>
@@ -1961,9 +2026,12 @@
         <v>0</v>
       </c>
       <c r="E8" s="11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F8" s="11">
+        <v>1</v>
+      </c>
+      <c r="G8" s="11">
         <v>1</v>
       </c>
     </row>
@@ -1974,54 +2042,56 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9AD2B396-A028-439B-AD56-80C88A7629A9}">
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="22.109375" style="12" customWidth="1"/>
-    <col min="2" max="2" width="18.44140625" customWidth="1"/>
-    <col min="3" max="3" width="19.77734375" customWidth="1"/>
-    <col min="4" max="4" width="20.44140625" customWidth="1"/>
-    <col min="5" max="5" width="20" customWidth="1"/>
-    <col min="6" max="6" width="12.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="35.21875" style="12" customWidth="1"/>
+    <col min="3" max="3" width="18.44140625" customWidth="1"/>
+    <col min="4" max="4" width="19.77734375" customWidth="1"/>
+    <col min="5" max="5" width="20.44140625" customWidth="1"/>
+    <col min="6" max="6" width="20" customWidth="1"/>
+    <col min="7" max="7" width="12.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>38</v>
       </c>
       <c r="B1" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="C1" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="D1" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="E1" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="F1" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="F1" s="13" t="s">
+      <c r="G1" s="13" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="B2">
-        <v>0</v>
+      <c r="B2" s="16" t="s">
+        <v>81</v>
       </c>
       <c r="C2">
         <v>0</v>
       </c>
       <c r="D2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E2">
         <v>1</v>
@@ -2029,13 +2099,16 @@
       <c r="F2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="B3">
-        <v>1</v>
+      <c r="B3" s="16" t="s">
+        <v>82</v>
       </c>
       <c r="C3">
         <v>1</v>
@@ -2049,16 +2122,19 @@
       <c r="F3">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="B4">
-        <v>0</v>
+      <c r="B4" s="16" t="s">
+        <v>83</v>
       </c>
       <c r="C4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D4">
         <v>1</v>
@@ -2069,19 +2145,22 @@
       <c r="F4">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="B5">
-        <v>0</v>
+      <c r="B5" s="17" t="s">
+        <v>85</v>
       </c>
       <c r="C5">
         <v>0</v>
       </c>
       <c r="D5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E5">
         <v>1</v>
@@ -2089,16 +2168,19 @@
       <c r="F5">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="B6">
-        <v>0</v>
+      <c r="B6" s="16" t="s">
+        <v>84</v>
       </c>
       <c r="C6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D6">
         <v>1</v>
@@ -2109,16 +2191,19 @@
       <c r="F6">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="B7">
-        <v>0</v>
+      <c r="B7" s="17" t="s">
+        <v>86</v>
       </c>
       <c r="C7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D7">
         <v>1</v>
@@ -2129,19 +2214,22 @@
       <c r="F7">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="B8">
-        <v>0</v>
+      <c r="B8" s="17" t="s">
+        <v>87</v>
       </c>
       <c r="C8">
         <v>0</v>
       </c>
       <c r="D8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E8">
         <v>1</v>
@@ -2149,19 +2237,22 @@
       <c r="F8">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="B9">
-        <v>0</v>
+      <c r="B9" s="17" t="s">
+        <v>88</v>
       </c>
       <c r="C9">
         <v>0</v>
       </c>
       <c r="D9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E9">
         <v>1</v>
@@ -2169,13 +2260,16 @@
       <c r="F9">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="12" t="s">
         <v>79</v>
       </c>
-      <c r="B10">
-        <v>0</v>
+      <c r="B10" s="17" t="s">
+        <v>89</v>
       </c>
       <c r="C10">
         <v>0</v>
@@ -2184,9 +2278,12 @@
         <v>0</v>
       </c>
       <c r="E10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F10">
+        <v>1</v>
+      </c>
+      <c r="G10">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
🛠 Julio 8 - 5
</commit_message>
<xml_diff>
--- a/data/Parametros.xlsx
+++ b/data/Parametros.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\00-OneDrive\OneDrive\99-DESARROLLO\Python\DataSmartExpress\App_DataSmart_Express\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/1510d6d17ff2404d/99-DESARROLLO/Python/DataSmartExpress/App_DataSmart_Express/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B72BE30E-4700-4877-934F-EAACCF4CDCCF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="17" documentId="13_ncr:1_{B72BE30E-4700-4877-934F-EAACCF4CDCCF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C4DCF0DB-C569-4D54-90C7-8383B1FE330B}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="1" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="KPIS_FINANCIEROS" sheetId="2" r:id="rId1"/>
@@ -19,6 +19,7 @@
     <sheet name="TARJETAS" sheetId="3" r:id="rId4"/>
     <sheet name="EN_ANALISIS" sheetId="6" r:id="rId5"/>
     <sheet name="PLANES" sheetId="4" r:id="rId6"/>
+    <sheet name="PLANES_INFO" sheetId="8" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="102">
   <si>
     <t>GRUPO</t>
   </si>
@@ -323,6 +324,27 @@
   </si>
   <si>
     <t>Tendencias 3 - 6 meses</t>
+  </si>
+  <si>
+    <t>PLAN</t>
+  </si>
+  <si>
+    <t>PRECIO_USD</t>
+  </si>
+  <si>
+    <t>DURACION_DIAS</t>
+  </si>
+  <si>
+    <t>DESCRIPCION CORTA</t>
+  </si>
+  <si>
+    <t>Análisis básico con indicadores clave</t>
+  </si>
+  <si>
+    <t>Todo el análisis avanzado + exportaciones</t>
+  </si>
+  <si>
+    <t>IA + gráficos inteligentes + comparativos</t>
   </si>
 </sst>
 </file>
@@ -414,7 +436,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -457,10 +479,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2044,7 +2062,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9AD2B396-A028-439B-AD56-80C88A7629A9}">
   <dimension ref="A1:G10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -2084,7 +2102,7 @@
       <c r="A2" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="B2" s="16" t="s">
+      <c r="B2" s="9" t="s">
         <v>81</v>
       </c>
       <c r="C2">
@@ -2107,7 +2125,7 @@
       <c r="A3" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="B3" s="16" t="s">
+      <c r="B3" s="9" t="s">
         <v>82</v>
       </c>
       <c r="C3">
@@ -2130,7 +2148,7 @@
       <c r="A4" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="B4" s="16" t="s">
+      <c r="B4" s="9" t="s">
         <v>83</v>
       </c>
       <c r="C4">
@@ -2153,7 +2171,7 @@
       <c r="A5" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="B5" s="17" t="s">
+      <c r="B5" t="s">
         <v>85</v>
       </c>
       <c r="C5">
@@ -2176,7 +2194,7 @@
       <c r="A6" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="B6" s="16" t="s">
+      <c r="B6" s="9" t="s">
         <v>84</v>
       </c>
       <c r="C6">
@@ -2199,7 +2217,7 @@
       <c r="A7" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="B7" s="17" t="s">
+      <c r="B7" t="s">
         <v>86</v>
       </c>
       <c r="C7">
@@ -2222,7 +2240,7 @@
       <c r="A8" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="B8" s="17" t="s">
+      <c r="B8" t="s">
         <v>87</v>
       </c>
       <c r="C8">
@@ -2245,7 +2263,7 @@
       <c r="A9" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="B9" s="17" t="s">
+      <c r="B9" t="s">
         <v>88</v>
       </c>
       <c r="C9">
@@ -2268,7 +2286,7 @@
       <c r="A10" s="12" t="s">
         <v>79</v>
       </c>
-      <c r="B10" s="17" t="s">
+      <c r="B10" t="s">
         <v>89</v>
       </c>
       <c r="C10">
@@ -2291,4 +2309,79 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4AF53A0-AAAF-49E4-B55C-40EF6F6F5FDC}">
+  <dimension ref="A1:D4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="36" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="8.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.21875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="35.5546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="B2" s="9">
+        <v>4.99</v>
+      </c>
+      <c r="C2" s="9">
+        <v>30</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="B3" s="9">
+        <v>9.99</v>
+      </c>
+      <c r="C3" s="9">
+        <v>30</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="B4" s="9">
+        <v>19.989999999999998</v>
+      </c>
+      <c r="C4" s="9">
+        <v>30</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>101</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
🛠 Julio 8 - 10
</commit_message>
<xml_diff>
--- a/data/Parametros.xlsx
+++ b/data/Parametros.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/1510d6d17ff2404d/99-DESARROLLO/Python/DataSmartExpress/App_DataSmart_Express/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="17" documentId="13_ncr:1_{B72BE30E-4700-4877-934F-EAACCF4CDCCF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C4DCF0DB-C569-4D54-90C7-8383B1FE330B}"/>
+  <xr:revisionPtr revIDLastSave="25" documentId="13_ncr:1_{B72BE30E-4700-4877-934F-EAACCF4CDCCF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8BDE58C8-3752-4E2B-AEBE-7D24876F1A6D}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="1" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="104">
   <si>
     <t>GRUPO</t>
   </si>
@@ -329,9 +329,6 @@
     <t>PLAN</t>
   </si>
   <si>
-    <t>PRECIO_USD</t>
-  </si>
-  <si>
     <t>DURACION_DIAS</t>
   </si>
   <si>
@@ -341,10 +338,19 @@
     <t>Análisis básico con indicadores clave</t>
   </si>
   <si>
-    <t>Todo el análisis avanzado + exportaciones</t>
-  </si>
-  <si>
-    <t>IA + gráficos inteligentes + comparativos</t>
+    <t>PRECIO</t>
+  </si>
+  <si>
+    <t>COP</t>
+  </si>
+  <si>
+    <t>USD</t>
+  </si>
+  <si>
+    <t>IA + exportaciones + análisis comparativo</t>
+  </si>
+  <si>
+    <t>IA avanzada + gráficas inteligentes</t>
   </si>
 </sst>
 </file>
@@ -436,7 +442,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -478,6 +484,10 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2313,72 +2323,85 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4AF53A0-AAAF-49E4-B55C-40EF6F6F5FDC}">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="36" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="8.21875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.77734375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.21875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="35.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="15.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" s="8" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" s="17" t="s">
         <v>95</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="17" t="s">
+        <v>99</v>
+      </c>
+      <c r="C1" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="D1" s="17" t="s">
         <v>96</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="E1" s="17" t="s">
         <v>97</v>
       </c>
-      <c r="D1" s="8" t="s">
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="B2" s="16">
+        <v>19900</v>
+      </c>
+      <c r="C2" s="16" t="s">
+        <v>100</v>
+      </c>
+      <c r="D2" s="16">
+        <v>30</v>
+      </c>
+      <c r="E2" s="16" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" s="9" t="s">
-        <v>41</v>
-      </c>
-      <c r="B2" s="9">
-        <v>4.99</v>
-      </c>
-      <c r="C2" s="9">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" s="16" t="s">
+        <v>42</v>
+      </c>
+      <c r="B3" s="16">
+        <v>9.99</v>
+      </c>
+      <c r="C3" s="16" t="s">
+        <v>101</v>
+      </c>
+      <c r="D3" s="16">
         <v>30</v>
       </c>
-      <c r="D2" s="9" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="B3" s="9">
-        <v>9.99</v>
-      </c>
-      <c r="C3" s="9">
+      <c r="E3" s="16" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" s="16" t="s">
+        <v>43</v>
+      </c>
+      <c r="B4" s="16">
+        <v>19.989999999999998</v>
+      </c>
+      <c r="C4" s="16" t="s">
+        <v>101</v>
+      </c>
+      <c r="D4" s="16">
         <v>30</v>
       </c>
-      <c r="D3" s="9" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="B4" s="9">
-        <v>19.989999999999998</v>
-      </c>
-      <c r="C4" s="9">
-        <v>30</v>
-      </c>
-      <c r="D4" s="9" t="s">
-        <v>101</v>
+      <c r="E4" s="16" t="s">
+        <v>103</v>
       </c>
     </row>
   </sheetData>

</xml_diff>